<commit_message>
Added two test caseb create and delete jira several dashboards by iterate a object array list of dashboard names via an ExcelDataProvider.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/developer_info.xlsx
+++ b/src/test/resources/data/developer_info.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\starter-project\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\school\ucsd-ext-jira1\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FFAEC2-5920-4CF4-8014-6FE372AED233}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19125" windowHeight="6930"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
-    <sheet name="addresses" sheetId="2" r:id="rId2"/>
+    <sheet name="animals" sheetId="3" r:id="rId2"/>
+    <sheet name="addresses" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>123 Oak Street</t>
   </si>
@@ -55,12 +57,33 @@
   </si>
   <si>
     <t>address_2</t>
+  </si>
+  <si>
+    <t>Armadillo</t>
+  </si>
+  <si>
+    <t>Anteater</t>
+  </si>
+  <si>
+    <t>Akita</t>
+  </si>
+  <si>
+    <t>Albatross</t>
+  </si>
+  <si>
+    <t>animal</t>
+  </si>
+  <si>
+    <t>Alpaca</t>
+  </si>
+  <si>
+    <t>Anchovy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,11 +428,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,11 +464,62 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88778B7B-2E40-4542-A684-FC1EDF2CD350}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>